<commit_message>
lab meeting update 8/19
</commit_message>
<xml_diff>
--- a/lab_meeting/lab_meeting_calendar.xlsx
+++ b/lab_meeting/lab_meeting_calendar.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bcmedu-my.sharepoint.com/personal/u244834_bcm_edu/Documents/lab/websites/frankfort-lab/lab_meeting/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="14" documentId="8_{B3463328-A060-409B-801D-1A35AED95DBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EC8F259E-9382-4DD2-8171-E808E31AAD33}"/>
+  <xr:revisionPtr revIDLastSave="34" documentId="8_{B3463328-A060-409B-801D-1A35AED95DBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F4D95DB1-D3EB-4C77-B3F7-0CBE74F6B7B1}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{148D7F30-F220-420D-858E-D08D52631B38}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{148D7F30-F220-420D-858E-D08D52631B38}"/>
   </bookViews>
   <sheets>
     <sheet name="2025" sheetId="3" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="24">
   <si>
     <t>Date</t>
   </si>
@@ -83,9 +83,6 @@
     <t>Justin</t>
   </si>
   <si>
-    <t>Jordan</t>
-  </si>
-  <si>
     <t>Bastille Day!  Celebrate democracy with a lab lunch :D</t>
   </si>
   <si>
@@ -93,6 +90,24 @@
   </si>
   <si>
     <t>No lab meeting - labor day</t>
+  </si>
+  <si>
+    <t>Schuyler</t>
+  </si>
+  <si>
+    <t>Schuyler Presentation and lab cleaning</t>
+  </si>
+  <si>
+    <t>Joseph</t>
+  </si>
+  <si>
+    <t>Someone</t>
+  </si>
+  <si>
+    <t>Rotation student presentations</t>
+  </si>
+  <si>
+    <t>Practice qualifying exam</t>
   </si>
 </sst>
 </file>
@@ -488,23 +503,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75BA943D-9A62-40D0-B0BF-8802F5644FD8}">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.88671875" customWidth="1"/>
-    <col min="2" max="2" width="17.33203125" customWidth="1"/>
-    <col min="3" max="3" width="19.44140625" customWidth="1"/>
-    <col min="4" max="4" width="22.5546875" customWidth="1"/>
-    <col min="5" max="5" width="18.88671875" customWidth="1"/>
-    <col min="6" max="6" width="13.6640625" customWidth="1"/>
+    <col min="1" max="1" width="14.85546875" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" customWidth="1"/>
+    <col min="3" max="3" width="19.42578125" customWidth="1"/>
+    <col min="4" max="4" width="22.5703125" customWidth="1"/>
+    <col min="5" max="5" width="18.85546875" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -527,7 +542,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>45838</v>
       </c>
@@ -539,7 +554,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <f>A2+7</f>
         <v>45845</v>
@@ -553,10 +568,10 @@
         <v>1</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <f t="shared" ref="A4:A9" si="0">A3+7</f>
         <v>45852</v>
@@ -572,10 +587,10 @@
         <v>0</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <f t="shared" si="0"/>
         <v>45859</v>
@@ -594,7 +609,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <f t="shared" si="0"/>
         <v>45866</v>
@@ -610,7 +625,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <f t="shared" si="0"/>
         <v>45873</v>
@@ -624,10 +639,10 @@
         <v>1</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <f t="shared" si="0"/>
         <v>45880</v>
@@ -641,10 +656,10 @@
         <v>1</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <f t="shared" si="0"/>
         <v>45887</v>
@@ -660,12 +675,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>45894</v>
       </c>
       <c r="B10" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="E10" t="s">
         <v>12</v>
@@ -674,8 +689,11 @@
         <f>FALSE</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <f>A10+7</f>
         <v>45901</v>
@@ -689,10 +707,10 @@
         <v>1</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <f t="shared" ref="A12:A16" si="1">A11+7</f>
         <v>45908</v>
@@ -708,13 +726,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <f t="shared" si="1"/>
         <v>45915</v>
       </c>
-      <c r="C13" t="s">
-        <v>14</v>
+      <c r="B13" t="s">
+        <v>20</v>
       </c>
       <c r="E13" t="s">
         <v>13</v>
@@ -723,53 +741,99 @@
         <f>FALSE</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <f t="shared" si="1"/>
         <v>45922</v>
       </c>
-      <c r="B14" t="s">
-        <v>7</v>
+      <c r="C14" t="s">
+        <v>14</v>
       </c>
       <c r="E14" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="F14" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <f t="shared" si="1"/>
         <v>45929</v>
       </c>
       <c r="B15" t="s">
+        <v>7</v>
+      </c>
+      <c r="E15" t="s">
         <v>14</v>
       </c>
-      <c r="E15" t="s">
-        <v>7</v>
-      </c>
       <c r="F15" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <f t="shared" si="1"/>
         <v>45936</v>
       </c>
       <c r="B16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E16" t="s">
+        <v>7</v>
+      </c>
+      <c r="F16" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>45943</v>
+      </c>
+      <c r="B17" t="s">
+        <v>12</v>
+      </c>
+      <c r="E17" t="s">
         <v>14</v>
       </c>
-      <c r="F16" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+      <c r="F17" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="G17" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
+        <v>45950</v>
+      </c>
+      <c r="B18" t="s">
+        <v>9</v>
+      </c>
+      <c r="E18" t="s">
+        <v>12</v>
+      </c>
+      <c r="F18" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
+        <v>45957</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
+        <v>45964</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
2025-09-08 lab meeting update
</commit_message>
<xml_diff>
--- a/lab_meeting/lab_meeting_calendar.xlsx
+++ b/lab_meeting/lab_meeting_calendar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bcmedu-my.sharepoint.com/personal/u244834_bcm_edu/Documents/lab/websites/frankfort-lab/lab_meeting/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="51" documentId="8_{B3463328-A060-409B-801D-1A35AED95DBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{19C367C6-5B0A-4E54-89B3-232B6370159D}"/>
+  <xr:revisionPtr revIDLastSave="66" documentId="8_{B3463328-A060-409B-801D-1A35AED95DBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6DA60F80-B91A-4CB7-BF96-4606F969FF36}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{148D7F30-F220-420D-858E-D08D52631B38}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="26">
   <si>
     <t>Date</t>
   </si>
@@ -101,9 +101,6 @@
     <t>Someone</t>
   </si>
   <si>
-    <t>Rotation student presentations</t>
-  </si>
-  <si>
     <t>Practice qualifying exam</t>
   </si>
   <si>
@@ -114,6 +111,9 @@
   </si>
   <si>
     <t>Schuyler virtual presentation and lab cleaning</t>
+  </si>
+  <si>
+    <t>Rotation student presentation &amp; happy hour. Starts at 3:00pm</t>
   </si>
 </sst>
 </file>
@@ -157,12 +157,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -497,10 +495,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75BA943D-9A62-40D0-B0BF-8802F5644FD8}">
-  <dimension ref="A1:H28"/>
+  <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -513,7 +511,7 @@
     <col min="6" max="6" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -536,390 +534,309 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
         <v>45838</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
+      <c r="F2" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
         <f>A2+7</f>
         <v>45845</v>
       </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="G3" s="4" t="s">
+      <c r="F3" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="G3" t="s">
         <v>16</v>
       </c>
-      <c r="H3" s="4"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
         <f t="shared" ref="A4:A9" si="0">A3+7</f>
         <v>45852</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4" t="s">
+      <c r="E4" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="4" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="G4" s="4" t="s">
+      <c r="F4" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="G4" t="s">
         <v>15</v>
       </c>
-      <c r="H4" s="4"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
         <f t="shared" si="0"/>
         <v>45859</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4" t="s">
+      <c r="E5" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="4" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="G5" s="4" t="s">
+      <c r="F5" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="G5" t="s">
         <v>11</v>
       </c>
-      <c r="H5" s="4"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
         <f t="shared" si="0"/>
         <v>45866</v>
       </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4" t="s">
+      <c r="C6" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4" t="s">
+      <c r="E6" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="4" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
+      <c r="F6" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
         <f t="shared" si="0"/>
         <v>45873</v>
       </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="G7" s="4" t="s">
+      <c r="F7" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="G7" t="s">
         <v>16</v>
       </c>
-      <c r="H7" s="4"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
         <f t="shared" si="0"/>
         <v>45880</v>
       </c>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="G8" s="4" t="s">
+      <c r="F8" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="G8" t="s">
         <v>16</v>
       </c>
-      <c r="H8" s="4"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="3">
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
         <f t="shared" si="0"/>
         <v>45887</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4" t="s">
+      <c r="E9" t="s">
         <v>9</v>
       </c>
-      <c r="F9" s="4" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="3">
+      <c r="F9" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
         <v>45894</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4" t="s">
+      <c r="E10" t="s">
         <v>12</v>
       </c>
-      <c r="F10" s="4" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="H10" s="4"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="3">
+      <c r="F10" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="G10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
         <f>A10+7</f>
         <v>45901</v>
       </c>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="G11" s="4" t="s">
+      <c r="F11" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="G11" t="s">
         <v>17</v>
       </c>
-      <c r="H11" s="4"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="3">
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
         <f t="shared" ref="A12:A16" si="1">A11+7</f>
         <v>45908</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4" t="s">
+      <c r="E12" t="s">
         <v>9</v>
       </c>
-      <c r="F12" s="4" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="3">
+      <c r="F12" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
         <f t="shared" si="1"/>
         <v>45915</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="C13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E13" t="s">
+        <v>13</v>
+      </c>
+      <c r="F13" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>45926</v>
+      </c>
+      <c r="B14" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F13" s="4" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="H13" s="4"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="3">
-        <f t="shared" si="1"/>
-        <v>45922</v>
-      </c>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4" t="s">
+      <c r="E14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="G14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <v>45929</v>
+      </c>
+      <c r="C15" t="s">
         <v>14</v>
       </c>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4" t="s">
+      <c r="E15" t="s">
         <v>20</v>
       </c>
-      <c r="F14" s="4" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="3">
-        <f t="shared" si="1"/>
-        <v>45929</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F15" s="4" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="3">
+      <c r="F15" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
         <f t="shared" si="1"/>
         <v>45936</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" t="s">
+        <v>7</v>
+      </c>
+      <c r="E16" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4" t="s">
+      <c r="F16" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>45943</v>
+      </c>
+      <c r="B17" t="s">
+        <v>14</v>
+      </c>
+      <c r="E17" t="s">
         <v>7</v>
       </c>
-      <c r="F16" s="4" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="3">
-        <v>45943</v>
-      </c>
-      <c r="B17" s="4" t="s">
+      <c r="F17" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
+        <v>45950</v>
+      </c>
+      <c r="B18" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4" t="s">
+      <c r="E18" t="s">
         <v>14</v>
       </c>
-      <c r="F17" s="4" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="G17" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="H17" s="4"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="3">
-        <v>45950</v>
-      </c>
-      <c r="B18" s="4" t="s">
+      <c r="F18" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="G18" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
+        <v>45957</v>
+      </c>
+      <c r="B19" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4" t="s">
+      <c r="E19" t="s">
         <v>12</v>
       </c>
-      <c r="F18" s="4" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="G18" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="H18" s="4"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="3">
-        <v>45957</v>
-      </c>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="G19" s="4"/>
-      <c r="H19" s="4"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="3">
+      <c r="F19" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="G19" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
         <v>45964</v>
       </c>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="G20" s="4"/>
-      <c r="H20" s="4"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="3">
+      <c r="F20" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
         <v>45971</v>
       </c>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="G21" s="4"/>
-      <c r="H21" s="4"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F21" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>45978</v>
       </c>
@@ -928,7 +845,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>45985</v>
       </c>
@@ -937,7 +854,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>45992</v>
       </c>
@@ -946,7 +863,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>45999</v>
       </c>
@@ -955,7 +872,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>46006</v>
       </c>
@@ -964,7 +881,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>46013</v>
       </c>
@@ -973,10 +890,10 @@
         <v>0</v>
       </c>
       <c r="G27" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>46020</v>
       </c>
@@ -985,7 +902,7 @@
         <v>0</v>
       </c>
       <c r="G28" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
lab meeting update 10/15/25
</commit_message>
<xml_diff>
--- a/lab_meeting/lab_meeting_calendar.xlsx
+++ b/lab_meeting/lab_meeting_calendar.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bcmedu-my.sharepoint.com/personal/u244834_bcm_edu/Documents/lab/websites/frankfort-lab/lab_meeting/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="66" documentId="8_{B3463328-A060-409B-801D-1A35AED95DBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6DA60F80-B91A-4CB7-BF96-4606F969FF36}"/>
+  <xr:revisionPtr revIDLastSave="88" documentId="8_{B3463328-A060-409B-801D-1A35AED95DBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{915F3CAD-0CC9-4C10-B203-3BA5A78BA57B}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{148D7F30-F220-420D-858E-D08D52631B38}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{148D7F30-F220-420D-858E-D08D52631B38}"/>
   </bookViews>
   <sheets>
     <sheet name="2025" sheetId="3" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="31">
   <si>
     <t>Date</t>
   </si>
@@ -101,9 +101,6 @@
     <t>Someone</t>
   </si>
   <si>
-    <t>Practice qualifying exam</t>
-  </si>
-  <si>
     <t>No lab meeting - winter break</t>
   </si>
   <si>
@@ -114,6 +111,24 @@
   </si>
   <si>
     <t>Rotation student presentation &amp; happy hour. Starts at 3:00pm</t>
+  </si>
+  <si>
+    <t>No Lab Meeting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Practice qual talk </t>
+  </si>
+  <si>
+    <t>Everyone</t>
+  </si>
+  <si>
+    <t>ARVO abstract talks</t>
+  </si>
+  <si>
+    <t>Joy, Giselle, Kevin.  Ben at AAO</t>
+  </si>
+  <si>
+    <t>Undergrads</t>
   </si>
 </sst>
 </file>
@@ -498,20 +513,21 @@
   <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" customWidth="1"/>
-    <col min="3" max="3" width="19.42578125" customWidth="1"/>
-    <col min="4" max="4" width="22.5703125" customWidth="1"/>
-    <col min="5" max="5" width="18.85546875" customWidth="1"/>
-    <col min="6" max="6" width="13.7109375" customWidth="1"/>
+    <col min="1" max="1" width="14.88671875" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" customWidth="1"/>
+    <col min="3" max="3" width="19.44140625" customWidth="1"/>
+    <col min="4" max="4" width="22.5546875" customWidth="1"/>
+    <col min="5" max="5" width="18.88671875" customWidth="1"/>
+    <col min="6" max="6" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -534,7 +550,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>45838</v>
       </c>
@@ -546,7 +562,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <f>A2+7</f>
         <v>45845</v>
@@ -559,7 +575,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <f t="shared" ref="A4:A9" si="0">A3+7</f>
         <v>45852</v>
@@ -578,7 +594,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <f t="shared" si="0"/>
         <v>45859</v>
@@ -597,7 +613,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <f t="shared" si="0"/>
         <v>45866</v>
@@ -613,7 +629,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <f t="shared" si="0"/>
         <v>45873</v>
@@ -626,7 +642,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <f t="shared" si="0"/>
         <v>45880</v>
@@ -639,7 +655,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <f t="shared" si="0"/>
         <v>45887</v>
@@ -655,7 +671,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>45894</v>
       </c>
@@ -670,10 +686,10 @@
         <v>0</v>
       </c>
       <c r="G10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <f>A10+7</f>
         <v>45901</v>
@@ -686,7 +702,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <f t="shared" ref="A12:A16" si="1">A11+7</f>
         <v>45908</v>
@@ -702,7 +718,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <f t="shared" si="1"/>
         <v>45915</v>
@@ -718,7 +734,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>45926</v>
       </c>
@@ -733,10 +749,10 @@
         <v>0</v>
       </c>
       <c r="G14" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>45929</v>
       </c>
@@ -751,7 +767,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <f t="shared" si="1"/>
         <v>45936</v>
@@ -767,12 +783,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>45943</v>
       </c>
       <c r="B17" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E17" t="s">
         <v>7</v>
@@ -781,31 +797,28 @@
         <f>FALSE</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G17" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>45950</v>
       </c>
-      <c r="B18" t="s">
-        <v>12</v>
-      </c>
-      <c r="E18" t="s">
-        <v>14</v>
-      </c>
       <c r="F18" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
       <c r="G18" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>45957</v>
       </c>
       <c r="B19" t="s">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="E19" t="s">
         <v>12</v>
@@ -815,28 +828,40 @@
         <v>0</v>
       </c>
       <c r="G19" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>45964</v>
       </c>
+      <c r="B20" t="s">
+        <v>27</v>
+      </c>
       <c r="F20" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G20" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>45971</v>
       </c>
+      <c r="B21" t="s">
+        <v>9</v>
+      </c>
       <c r="F21" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G21" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>45978</v>
       </c>
@@ -845,7 +870,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <v>45985</v>
       </c>
@@ -854,7 +879,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <v>45992</v>
       </c>
@@ -863,7 +888,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <v>45999</v>
       </c>
@@ -872,7 +897,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <v>46006</v>
       </c>
@@ -881,7 +906,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
         <v>46013</v>
       </c>
@@ -890,10 +915,10 @@
         <v>0</v>
       </c>
       <c r="G27" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <v>46020</v>
       </c>
@@ -902,7 +927,7 @@
         <v>0</v>
       </c>
       <c r="G28" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
10-27-25 lab meeting update
</commit_message>
<xml_diff>
--- a/lab_meeting/lab_meeting_calendar.xlsx
+++ b/lab_meeting/lab_meeting_calendar.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bcmedu-my.sharepoint.com/personal/u244834_bcm_edu/Documents/lab/websites/frankfort-lab/lab_meeting/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="88" documentId="8_{B3463328-A060-409B-801D-1A35AED95DBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{915F3CAD-0CC9-4C10-B203-3BA5A78BA57B}"/>
+  <xr:revisionPtr revIDLastSave="99" documentId="8_{B3463328-A060-409B-801D-1A35AED95DBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{948CBADE-3FCD-40CD-B381-D2FB3AE01FA4}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{148D7F30-F220-420D-858E-D08D52631B38}"/>
+    <workbookView xWindow="28680" yWindow="-5445" windowWidth="38640" windowHeight="21120" xr2:uid="{148D7F30-F220-420D-858E-D08D52631B38}"/>
   </bookViews>
   <sheets>
     <sheet name="2025" sheetId="3" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="34">
   <si>
     <t>Date</t>
   </si>
@@ -122,13 +122,22 @@
     <t>Everyone</t>
   </si>
   <si>
-    <t>ARVO abstract talks</t>
-  </si>
-  <si>
     <t>Joy, Giselle, Kevin.  Ben at AAO</t>
   </si>
   <si>
     <t>Undergrads</t>
+  </si>
+  <si>
+    <t>no meeting - Thanksgiving</t>
+  </si>
+  <si>
+    <t>ARVO abstract talks. Start at 10am</t>
+  </si>
+  <si>
+    <t>Solomon's PhD</t>
+  </si>
+  <si>
+    <t>ARVO abstract editing</t>
   </si>
 </sst>
 </file>
@@ -510,11 +519,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75BA943D-9A62-40D0-B0BF-8802F5644FD8}">
-  <dimension ref="A1:G28"/>
+  <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D21" sqref="D21"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -818,7 +827,7 @@
         <v>45957</v>
       </c>
       <c r="B19" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E19" t="s">
         <v>12</v>
@@ -828,7 +837,7 @@
         <v>0</v>
       </c>
       <c r="G19" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
@@ -843,7 +852,7 @@
         <v>0</v>
       </c>
       <c r="G20" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
@@ -865,6 +874,12 @@
       <c r="A22" s="2">
         <v>45978</v>
       </c>
+      <c r="B22" t="s">
+        <v>14</v>
+      </c>
+      <c r="E22" t="s">
+        <v>9</v>
+      </c>
       <c r="F22" t="b">
         <f>FALSE</f>
         <v>0</v>
@@ -872,34 +887,49 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
-        <v>45985</v>
+        <v>45981</v>
+      </c>
+      <c r="B23" t="s">
+        <v>9</v>
       </c>
       <c r="F23" t="b">
         <f>FALSE</f>
         <v>0</v>
+      </c>
+      <c r="G23" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
-        <v>45992</v>
+        <v>45985</v>
       </c>
       <c r="F24" t="b">
         <f>FALSE</f>
         <v>0</v>
+      </c>
+      <c r="G24" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
-        <v>45999</v>
+        <v>45992</v>
+      </c>
+      <c r="B25" t="s">
+        <v>27</v>
       </c>
       <c r="F25" t="b">
         <f>FALSE</f>
         <v>0</v>
+      </c>
+      <c r="G25" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
-        <v>46006</v>
+        <v>45999</v>
       </c>
       <c r="F26" t="b">
         <f>FALSE</f>
@@ -908,25 +938,34 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
-        <v>46013</v>
+        <v>46006</v>
       </c>
       <c r="F27" t="b">
         <f>FALSE</f>
         <v>0</v>
-      </c>
-      <c r="G27" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
+        <v>46013</v>
+      </c>
+      <c r="F28" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="G28" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A29" s="2">
         <v>46020</v>
       </c>
-      <c r="F28" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="G28" t="s">
+      <c r="F29" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="G29" t="s">
         <v>21</v>
       </c>
     </row>

</xml_diff>

<commit_message>
2026 lab meeting - part 1
</commit_message>
<xml_diff>
--- a/lab_meeting/lab_meeting_calendar.xlsx
+++ b/lab_meeting/lab_meeting_calendar.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bcmedu-my.sharepoint.com/personal/u244834_bcm_edu/Documents/lab/websites/frankfort-lab/lab_meeting/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="99" documentId="8_{B3463328-A060-409B-801D-1A35AED95DBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{948CBADE-3FCD-40CD-B381-D2FB3AE01FA4}"/>
+  <xr:revisionPtr revIDLastSave="162" documentId="8_{B3463328-A060-409B-801D-1A35AED95DBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F62E1F7D-A7EA-4095-92AF-7A1CCBB8E4DD}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-5445" windowWidth="38640" windowHeight="21120" xr2:uid="{148D7F30-F220-420D-858E-D08D52631B38}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{148D7F30-F220-420D-858E-D08D52631B38}"/>
   </bookViews>
   <sheets>
     <sheet name="2025" sheetId="3" r:id="rId1"/>
+    <sheet name="2026" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="57">
   <si>
     <t>Date</t>
   </si>
@@ -138,6 +139,75 @@
   </si>
   <si>
     <t>ARVO abstract editing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lab Planning </t>
+  </si>
+  <si>
+    <t xml:space="preserve">MLK Day Volunteering </t>
+  </si>
+  <si>
+    <t>lab planning</t>
+  </si>
+  <si>
+    <t>no lab meeting</t>
+  </si>
+  <si>
+    <t>Ben out of town</t>
+  </si>
+  <si>
+    <t>spring break for Rice</t>
+  </si>
+  <si>
+    <t>Chantel George</t>
+  </si>
+  <si>
+    <t>Solomon Gibson</t>
+  </si>
+  <si>
+    <t>Guofu Shen</t>
+  </si>
+  <si>
+    <t>Daniel Brock</t>
+  </si>
+  <si>
+    <t>Justin Ma</t>
+  </si>
+  <si>
+    <t>lab farewell party for Justin</t>
+  </si>
+  <si>
+    <t>Lab vision / Frankfort lab retreat</t>
+  </si>
+  <si>
+    <t>Salim Khondker</t>
+  </si>
+  <si>
+    <t>Soumi Mitra</t>
+  </si>
+  <si>
+    <t>Rice finals</t>
+  </si>
+  <si>
+    <t>Kevin Wu</t>
+  </si>
+  <si>
+    <t>Giselle Gonzalez</t>
+  </si>
+  <si>
+    <t>Joy Kim</t>
+  </si>
+  <si>
+    <t>Daniel Brock (pilot)</t>
+  </si>
+  <si>
+    <t>Med Student Day</t>
+  </si>
+  <si>
+    <t>Reagan, Ritu, Miles, Molly, Grace</t>
+  </si>
+  <si>
+    <t>Ben Frankfort &amp; Daniel Brock</t>
   </si>
 </sst>
 </file>
@@ -521,22 +591,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75BA943D-9A62-40D0-B0BF-8802F5644FD8}">
   <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.88671875" customWidth="1"/>
-    <col min="2" max="2" width="17.33203125" customWidth="1"/>
-    <col min="3" max="3" width="19.44140625" customWidth="1"/>
-    <col min="4" max="4" width="22.5546875" customWidth="1"/>
-    <col min="5" max="5" width="18.88671875" customWidth="1"/>
-    <col min="6" max="6" width="13.6640625" customWidth="1"/>
+    <col min="1" max="1" width="14.85546875" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" customWidth="1"/>
+    <col min="3" max="3" width="19.42578125" customWidth="1"/>
+    <col min="4" max="4" width="22.5703125" customWidth="1"/>
+    <col min="5" max="5" width="18.85546875" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -559,7 +629,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>45838</v>
       </c>
@@ -571,7 +641,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <f>A2+7</f>
         <v>45845</v>
@@ -584,7 +654,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <f t="shared" ref="A4:A9" si="0">A3+7</f>
         <v>45852</v>
@@ -603,7 +673,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <f t="shared" si="0"/>
         <v>45859</v>
@@ -622,7 +692,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <f t="shared" si="0"/>
         <v>45866</v>
@@ -638,7 +708,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <f t="shared" si="0"/>
         <v>45873</v>
@@ -651,7 +721,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <f t="shared" si="0"/>
         <v>45880</v>
@@ -664,7 +734,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <f t="shared" si="0"/>
         <v>45887</v>
@@ -680,7 +750,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>45894</v>
       </c>
@@ -698,7 +768,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <f>A10+7</f>
         <v>45901</v>
@@ -711,7 +781,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <f t="shared" ref="A12:A16" si="1">A11+7</f>
         <v>45908</v>
@@ -727,7 +797,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <f t="shared" si="1"/>
         <v>45915</v>
@@ -743,7 +813,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>45926</v>
       </c>
@@ -761,7 +831,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>45929</v>
       </c>
@@ -776,7 +846,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <f t="shared" si="1"/>
         <v>45936</v>
@@ -792,7 +862,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>45943</v>
       </c>
@@ -810,7 +880,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>45950</v>
       </c>
@@ -822,7 +892,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>45957</v>
       </c>
@@ -840,7 +910,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>45964</v>
       </c>
@@ -855,7 +925,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>45971</v>
       </c>
@@ -870,7 +940,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>45978</v>
       </c>
@@ -885,7 +955,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>45981</v>
       </c>
@@ -900,7 +970,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>45985</v>
       </c>
@@ -912,7 +982,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>45992</v>
       </c>
@@ -927,7 +997,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>45999</v>
       </c>
@@ -936,7 +1006,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>46006</v>
       </c>
@@ -945,7 +1015,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>46013</v>
       </c>
@@ -957,7 +1027,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>46020</v>
       </c>
@@ -968,6 +1038,300 @@
       <c r="G29" t="s">
         <v>21</v>
       </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8914FEE5-3B14-4065-9F37-64FFCCDB3E85}">
+  <dimension ref="A1:F29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D16" sqref="D16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.85546875" customWidth="1"/>
+    <col min="2" max="2" width="27" customWidth="1"/>
+    <col min="3" max="3" width="19.42578125" customWidth="1"/>
+    <col min="4" max="4" width="18.85546875" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>46034</v>
+      </c>
+      <c r="B2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>46041</v>
+      </c>
+      <c r="B3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E3" t="b">
+        <v>0</v>
+      </c>
+      <c r="F3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>46048</v>
+      </c>
+      <c r="B4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E4" t="b">
+        <v>0</v>
+      </c>
+      <c r="F4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>46055</v>
+      </c>
+      <c r="B5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5" t="s">
+        <v>53</v>
+      </c>
+      <c r="E5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>46062</v>
+      </c>
+      <c r="B6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E6" t="b">
+        <v>0</v>
+      </c>
+      <c r="F6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>46069</v>
+      </c>
+      <c r="B7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" t="s">
+        <v>40</v>
+      </c>
+      <c r="E7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>46076</v>
+      </c>
+      <c r="B8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" t="s">
+        <v>47</v>
+      </c>
+      <c r="E8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>46083</v>
+      </c>
+      <c r="B9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" t="s">
+        <v>48</v>
+      </c>
+      <c r="E9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>46090</v>
+      </c>
+      <c r="B10" t="s">
+        <v>48</v>
+      </c>
+      <c r="C10" t="s">
+        <v>42</v>
+      </c>
+      <c r="E10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>46097</v>
+      </c>
+      <c r="B11" t="s">
+        <v>56</v>
+      </c>
+      <c r="E11" t="b">
+        <v>0</v>
+      </c>
+      <c r="F11" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>46104</v>
+      </c>
+      <c r="B12" t="s">
+        <v>54</v>
+      </c>
+      <c r="E12" t="b">
+        <v>0</v>
+      </c>
+      <c r="F12" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>46111</v>
+      </c>
+      <c r="B13" t="s">
+        <v>52</v>
+      </c>
+      <c r="E13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>46118</v>
+      </c>
+      <c r="B14" t="s">
+        <v>37</v>
+      </c>
+      <c r="E14" t="b">
+        <v>0</v>
+      </c>
+      <c r="F14" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <v>46125</v>
+      </c>
+      <c r="B15" t="s">
+        <v>50</v>
+      </c>
+      <c r="E15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <v>46132</v>
+      </c>
+      <c r="B16" t="s">
+        <v>51</v>
+      </c>
+      <c r="E16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>46139</v>
+      </c>
+      <c r="E17" t="b">
+        <v>0</v>
+      </c>
+      <c r="F17" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="2"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="2"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="2"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="2"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="2"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="2"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="2"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="2"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="2"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="2"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="2"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>